<commit_message>
Testing code now finished. Moved into live testing phase.
</commit_message>
<xml_diff>
--- a/config_files/1 - CDP Network Audit _ Template.xlsx
+++ b/config_files/1 - CDP Network Audit _ Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\PycharmProjects\AsyncSSH\config_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\PycharmProjects\CDP_Network_Map\config_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F63443-95FB-4CF4-8367-766047A8CA9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D545420-D3D6-4D68-99DB-0F4D74C05916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,19 +19,22 @@
     <sheet name="Authentication Errors" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Audit!$A$11:$I$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Audit!$A$11:$K$11</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'DNS Resolved'!$A$4:$B$4</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>CDP Device Audit</t>
   </si>
   <si>
+    <t>Site Code:</t>
+  </si>
+  <si>
     <t>Date:</t>
   </si>
   <si>
@@ -41,12 +44,12 @@
     <t>Seed Device 1:</t>
   </si>
   <si>
+    <t>10.145.63.1</t>
+  </si>
+  <si>
     <t>Seed Device 2:</t>
   </si>
   <si>
-    <t>Site Code:</t>
-  </si>
-  <si>
     <t>LOCAL_HOST</t>
   </si>
   <si>
@@ -74,32 +77,59 @@
     <t>CAPABILITIES</t>
   </si>
   <si>
+    <t>GB-CAY2-001CSW001</t>
+  </si>
+  <si>
+    <t>GB-CAY2-001ASW001</t>
+  </si>
+  <si>
+    <t>10.145.61.10</t>
+  </si>
+  <si>
+    <t>gb-cay2-001sdw101</t>
+  </si>
+  <si>
+    <t>gb-cay2-001sdw102</t>
+  </si>
+  <si>
+    <t>Reverse DNS Lookup</t>
+  </si>
+  <si>
+    <t>Hostname</t>
+  </si>
+  <si>
+    <t>IP Address</t>
+  </si>
+  <si>
+    <t>10.255.145.61</t>
+  </si>
+  <si>
+    <t>10.255.145.62</t>
+  </si>
+  <si>
+    <t>Connection Errors</t>
+  </si>
+  <si>
     <t>Authentication Errors</t>
   </si>
   <si>
-    <t>Hostname</t>
-  </si>
-  <si>
-    <t>IP Address</t>
-  </si>
-  <si>
-    <t>Connection Errors</t>
-  </si>
-  <si>
-    <t>DNS Resolved IP Addresses</t>
-  </si>
-  <si>
-    <t>LOCAL_SERIAL</t>
-  </si>
-  <si>
-    <t>LOCAL_UPTIME</t>
+    <t>LOCAL UPTIME</t>
+  </si>
+  <si>
+    <t>LOCAL SERIAL</t>
+  </si>
+  <si>
+    <t>Local Host Information</t>
+  </si>
+  <si>
+    <t>Remote Host Information</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,8 +153,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -155,8 +215,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -208,11 +278,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -250,42 +372,71 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -588,104 +739,147 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="6" width="30.6640625" customWidth="1"/>
-    <col min="7" max="7" width="50.6640625" customWidth="1"/>
-    <col min="8" max="8" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.6640625" customWidth="1"/>
-    <col min="10" max="10" width="109.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="50.6640625" customWidth="1"/>
+    <col min="5" max="5" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="30.6640625" customWidth="1"/>
+    <col min="10" max="10" width="108.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-    </row>
-    <row r="3" spans="1:11" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B4" s="4"/>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" s="4"/>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6" s="4"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7" s="4"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B8" s="4"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6"/>
       <c r="B9" s="4"/>
     </row>
+    <row r="10" spans="1:11" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="19"/>
+    </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="3" t="s">
+      <c r="A11" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="B11" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="3" t="s">
+      <c r="C11" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="D11" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="G11" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="H11" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="3" t="s">
+      <c r="I11" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="K11" s="3" t="s">
+      <c r="J11" s="13" t="s">
         <v>14</v>
       </c>
+      <c r="K11" s="13" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A11:I11" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <mergeCells count="2">
+  <autoFilter ref="A11:I11" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <mergeCells count="12">
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="F10:K10"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -693,11 +887,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF264A58-7302-43F4-8536-3DC3756319EC}">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -707,40 +901,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="15"/>
+      <c r="A1" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="25"/>
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="14"/>
-      <c r="B2" s="16"/>
-    </row>
-    <row r="3" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>17</v>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A4:B4" xr:uid="{CF264A58-7302-43F4-8536-3DC3756319EC}"/>
+  <autoFilter ref="A4:B4" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <mergeCells count="2">
+    <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
   </mergeCells>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="DNS Resolution Failed">
+      <formula>NOT(ISERROR(SEARCH("DNS Resolution Failed",B1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57BC569B-A16A-4198-9DB5-FADCB4818C57}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -749,19 +980,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="17"/>
+      <c r="A1" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="28"/>
     </row>
     <row r="2" spans="1:2" s="10" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-    </row>
-    <row r="3" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -773,11 +1004,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A1C2847-EC79-480E-B4B3-31C0E0F06CAB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -786,19 +1017,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="19"/>
+      <c r="A1" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="28"/>
     </row>
     <row r="2" spans="1:2" s="12" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-    </row>
-    <row r="3" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1. Added arguments parsing using argparse. 2. Modified Excel template file.
</commit_message>
<xml_diff>
--- a/config_files/1 - CDP Network Audit _ Template.xlsx
+++ b/config_files/1 - CDP Network Audit _ Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\PycharmProjects\CDP_Network_Map\config_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\PycharmProjects\AsyncSSH\config_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D545420-D3D6-4D68-99DB-0F4D74C05916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D14995-A9D6-47B2-B300-E4CCC6301CF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>CDP Device Audit</t>
   </si>
@@ -41,15 +41,9 @@
     <t>Time:</t>
   </si>
   <si>
-    <t>Seed Device 1:</t>
-  </si>
-  <si>
     <t>10.145.63.1</t>
   </si>
   <si>
-    <t>Seed Device 2:</t>
-  </si>
-  <si>
     <t>LOCAL_HOST</t>
   </si>
   <si>
@@ -123,6 +117,9 @@
   </si>
   <si>
     <t>Remote Host Information</t>
+  </si>
+  <si>
+    <t>Seed Device:</t>
   </si>
 </sst>
 </file>
@@ -739,7 +736,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -799,14 +796,12 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B7" s="4"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>6</v>
-      </c>
+      <c r="A8" s="6"/>
       <c r="B8" s="4"/>
     </row>
     <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -815,14 +810,14 @@
     </row>
     <row r="10" spans="1:11" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
       <c r="E10" s="16"/>
       <c r="F10" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G10" s="18"/>
       <c r="H10" s="18"/>
@@ -832,37 +827,37 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="D11" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="G11" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" s="13" t="s">
+      <c r="H11" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="I11" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="13" t="s">
+      <c r="J11" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="13" t="s">
+      <c r="K11" s="13" t="s">
         <v>13</v>
-      </c>
-      <c r="J11" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="K11" s="13" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -902,7 +897,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B1" s="25"/>
     </row>
@@ -913,42 +908,42 @@
     <row r="3" spans="1:2" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -981,7 +976,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="27" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B1" s="28"/>
     </row>
@@ -992,7 +987,7 @@
     <row r="3" spans="1:2" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1018,7 +1013,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="29" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B1" s="28"/>
     </row>
@@ -1029,7 +1024,7 @@
     <row r="3" spans="1:2" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>